<commit_message>
Added a program to calculate reaction coordinate using ideal gas and equilibrium constant. Fixed issues with the original equilibrium constant program. Updated database, added properties of pure species (for future use in reaction coordinate calculations with non-ideal conditions).
</commit_message>
<xml_diff>
--- a/Heat_Capacity_Poly_Database.xlsx
+++ b/Heat_Capacity_Poly_Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Adal\IBERO\S5\EQQ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Adal\IBERO\S5\EQQ\Equilibrium-Constant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A847FE95-09EE-4888-B7BA-51293EC9F364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF0A294-9C43-45B0-A170-145E4CCAA8D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Heat Capacities" sheetId="1" r:id="rId1"/>
@@ -29,206 +29,83 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="224">
   <si>
     <t>Methane</t>
   </si>
   <si>
-    <t>CH4</t>
-  </si>
-  <si>
     <t>Ethane</t>
   </si>
   <si>
-    <t>C2H6</t>
-  </si>
-  <si>
     <t>Propane</t>
   </si>
   <si>
-    <t>C3H8</t>
-  </si>
-  <si>
-    <t>C4H10</t>
-  </si>
-  <si>
-    <t>C5H12</t>
-  </si>
-  <si>
-    <t>C6H14</t>
-  </si>
-  <si>
-    <t>C7H16</t>
-  </si>
-  <si>
-    <t>C8H18</t>
-  </si>
-  <si>
-    <t>C2H4</t>
-  </si>
-  <si>
     <t>Propylene</t>
   </si>
   <si>
-    <t>C3H6</t>
-  </si>
-  <si>
-    <t>C4H8</t>
-  </si>
-  <si>
-    <t>C5H10</t>
-  </si>
-  <si>
-    <t>C6H12</t>
-  </si>
-  <si>
-    <t>C7H14</t>
-  </si>
-  <si>
-    <t>C8H16</t>
-  </si>
-  <si>
     <t>Acetaldehyde</t>
   </si>
   <si>
-    <t>C2H4O</t>
-  </si>
-  <si>
     <t>Acetylene</t>
   </si>
   <si>
-    <t>C2H2</t>
-  </si>
-  <si>
     <t>Benzene</t>
   </si>
   <si>
-    <t>C6H6</t>
-  </si>
-  <si>
     <t>1,3-Butadiene</t>
   </si>
   <si>
-    <t>C4H6</t>
-  </si>
-  <si>
     <t>Cyclohexane</t>
   </si>
   <si>
     <t>Ethanol</t>
   </si>
   <si>
-    <t>C2H6O</t>
-  </si>
-  <si>
     <t>Ethylbenzene</t>
   </si>
   <si>
-    <t>C8H10</t>
-  </si>
-  <si>
     <t>Formaldehyde</t>
   </si>
   <si>
-    <t>CH2O</t>
-  </si>
-  <si>
     <t>Methanol</t>
   </si>
   <si>
-    <t>CH4O</t>
-  </si>
-  <si>
     <t>Styrene</t>
   </si>
   <si>
-    <t>C8H8</t>
-  </si>
-  <si>
     <t>Toluene</t>
   </si>
   <si>
-    <t>C7H8</t>
-  </si>
-  <si>
     <t>Air</t>
   </si>
   <si>
     <t>Ammonia</t>
   </si>
   <si>
-    <t>NH3</t>
-  </si>
-  <si>
     <t>Bromine</t>
   </si>
   <si>
-    <t>Br2</t>
-  </si>
-  <si>
     <t>CO</t>
   </si>
   <si>
-    <t>CO2</t>
-  </si>
-  <si>
-    <t>CS2</t>
-  </si>
-  <si>
     <t>Chlorine</t>
   </si>
   <si>
-    <t>Cl2</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>H2S</t>
-  </si>
-  <si>
     <t>HCl</t>
   </si>
   <si>
     <t>HCN</t>
   </si>
   <si>
-    <t>Nitrogen</t>
-  </si>
-  <si>
-    <t>N2</t>
-  </si>
-  <si>
-    <t>N2O</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
-    <t>NO2</t>
-  </si>
-  <si>
-    <t>N2O4</t>
-  </si>
-  <si>
     <t>Oxygen</t>
   </si>
   <si>
-    <t>O2</t>
-  </si>
-  <si>
-    <t>SO2</t>
-  </si>
-  <si>
-    <t>SO3</t>
-  </si>
-  <si>
     <t>Water</t>
   </si>
   <si>
-    <t>H2O</t>
-  </si>
-  <si>
     <t>Ethylene oxide</t>
   </si>
   <si>
@@ -503,6 +380,327 @@
   </si>
   <si>
     <t>Ethylene_(gas)</t>
+  </si>
+  <si>
+    <t>C_4H_6</t>
+  </si>
+  <si>
+    <t>C_4H_8</t>
+  </si>
+  <si>
+    <t>C_2H_2</t>
+  </si>
+  <si>
+    <t>(O_2+3.74N_2)</t>
+  </si>
+  <si>
+    <t>Br_2</t>
+  </si>
+  <si>
+    <t>CO_2</t>
+  </si>
+  <si>
+    <t>CS_2</t>
+  </si>
+  <si>
+    <t>Cl_2</t>
+  </si>
+  <si>
+    <t>CH_2O</t>
+  </si>
+  <si>
+    <t>H_2</t>
+  </si>
+  <si>
+    <t>H_2S</t>
+  </si>
+  <si>
+    <t>N_2</t>
+  </si>
+  <si>
+    <t>NO_2</t>
+  </si>
+  <si>
+    <t>N_2O</t>
+  </si>
+  <si>
+    <t>O_2</t>
+  </si>
+  <si>
+    <t>SO_2</t>
+  </si>
+  <si>
+    <t>H_2O</t>
+  </si>
+  <si>
+    <t>NH_3</t>
+  </si>
+  <si>
+    <t>SO_3</t>
+  </si>
+  <si>
+    <t>C_2H_4O</t>
+  </si>
+  <si>
+    <t>N_2O_4</t>
+  </si>
+  <si>
+    <t>C_2H_4</t>
+  </si>
+  <si>
+    <t>CH_4</t>
+  </si>
+  <si>
+    <t>CH_4O</t>
+  </si>
+  <si>
+    <t>C_8H_16</t>
+  </si>
+  <si>
+    <t>C_6H1_2</t>
+  </si>
+  <si>
+    <t>C_6H_6</t>
+  </si>
+  <si>
+    <t>C_2H_6</t>
+  </si>
+  <si>
+    <t>C_2H_6O</t>
+  </si>
+  <si>
+    <t>C_3H_6</t>
+  </si>
+  <si>
+    <t>C_5H_10</t>
+  </si>
+  <si>
+    <t>C_6H_12</t>
+  </si>
+  <si>
+    <t>C_8H_10</t>
+  </si>
+  <si>
+    <t>C_7H1_4</t>
+  </si>
+  <si>
+    <t>C_4H_10</t>
+  </si>
+  <si>
+    <t>C_7H_16</t>
+  </si>
+  <si>
+    <t>C_6H_14</t>
+  </si>
+  <si>
+    <t>C_8H_18</t>
+  </si>
+  <si>
+    <t>C_5H_12</t>
+  </si>
+  <si>
+    <t>C_3H_8</t>
+  </si>
+  <si>
+    <t>C_8H_8</t>
+  </si>
+  <si>
+    <t>C_7H_8</t>
+  </si>
+  <si>
+    <t>Nitrogen_(gas)</t>
+  </si>
+  <si>
+    <t>n-Butane</t>
+  </si>
+  <si>
+    <t>n-Pentane</t>
+  </si>
+  <si>
+    <t>n-Hexane</t>
+  </si>
+  <si>
+    <t>n-Heptane</t>
+  </si>
+  <si>
+    <t>n-Octane</t>
+  </si>
+  <si>
+    <t>n-Nonane</t>
+  </si>
+  <si>
+    <t>n-Decane</t>
+  </si>
+  <si>
+    <t>Isobutane</t>
+  </si>
+  <si>
+    <t>Isooctane</t>
+  </si>
+  <si>
+    <t>Zc</t>
+  </si>
+  <si>
+    <t>Vc</t>
+  </si>
+  <si>
+    <t>Molar mass</t>
+  </si>
+  <si>
+    <t>omega</t>
+  </si>
+  <si>
+    <t>Tc</t>
+  </si>
+  <si>
+    <t>Pc</t>
+  </si>
+  <si>
+    <t>Tn</t>
+  </si>
+  <si>
+    <t>Cyclopentane</t>
+  </si>
+  <si>
+    <t>Methylcyclopentane</t>
+  </si>
+  <si>
+    <t>Methylcyclohexane</t>
+  </si>
+  <si>
+    <t>Ethylene</t>
+  </si>
+  <si>
+    <t>1-Butene</t>
+  </si>
+  <si>
+    <t>cis-2-Butene</t>
+  </si>
+  <si>
+    <t>trans-2-Butene</t>
+  </si>
+  <si>
+    <t>1-Hexene</t>
+  </si>
+  <si>
+    <t>Isobutylene</t>
+  </si>
+  <si>
+    <t>Cyclohexene</t>
+  </si>
+  <si>
+    <t>Cumene</t>
+  </si>
+  <si>
+    <t>o-Xylene</t>
+  </si>
+  <si>
+    <t>m-Xylene</t>
+  </si>
+  <si>
+    <t>p-Xylene</t>
+  </si>
+  <si>
+    <t>Naphthalene</t>
+  </si>
+  <si>
+    <t>Biphenyl</t>
+  </si>
+  <si>
+    <t>Acetone</t>
+  </si>
+  <si>
+    <t>1-Propanol</t>
+  </si>
+  <si>
+    <t>1-Butanol</t>
+  </si>
+  <si>
+    <t>1-Hexanol</t>
+  </si>
+  <si>
+    <t>2-Propanol</t>
+  </si>
+  <si>
+    <t>Phenol</t>
+  </si>
+  <si>
+    <t>Acetonitrile</t>
+  </si>
+  <si>
+    <t>Methylamine</t>
+  </si>
+  <si>
+    <t>Ethylamine</t>
+  </si>
+  <si>
+    <t>Nitromethane</t>
+  </si>
+  <si>
+    <t>Dichloromethane</t>
+  </si>
+  <si>
+    <t>Tetrafluoroethane</t>
+  </si>
+  <si>
+    <t>Argon</t>
+  </si>
+  <si>
+    <t>Krypton</t>
+  </si>
+  <si>
+    <t>Xenon</t>
+  </si>
+  <si>
+    <t>−0.390</t>
+  </si>
+  <si>
+    <t>−0.216</t>
+  </si>
+  <si>
+    <t>Methyl_acetate</t>
+  </si>
+  <si>
+    <t>Ethyl_acetate</t>
+  </si>
+  <si>
+    <t>Methyl_ethyl_ketone</t>
+  </si>
+  <si>
+    <t>Diethyl_ether</t>
+  </si>
+  <si>
+    <t>Methyl_t-butyl_ether</t>
+  </si>
+  <si>
+    <t>Ethylene_glycol</t>
+  </si>
+  <si>
+    <t>Acetic_acid</t>
+  </si>
+  <si>
+    <t>n-Butyric_acid</t>
+  </si>
+  <si>
+    <t>Benzoic_acid</t>
+  </si>
+  <si>
+    <t>Carbon_tetrachloride</t>
+  </si>
+  <si>
+    <t>Methyl_chloride</t>
+  </si>
+  <si>
+    <t>Ethyl_chloride</t>
+  </si>
+  <si>
+    <t>Helium_4</t>
+  </si>
+  <si>
+    <t>Nitric_acid</t>
+  </si>
+  <si>
+    <t>Sulfuric_acid</t>
   </si>
 </sst>
 </file>
@@ -510,7 +708,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -541,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -554,10 +752,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -840,9 +1039,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A23" sqref="A23"/>
+      <selection pane="topRight" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,10 +1061,10 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="C1" s="6">
         <v>1500</v>
@@ -892,10 +1091,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="C2" s="6">
         <v>1500</v>
@@ -922,10 +1121,10 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>150</v>
       </c>
       <c r="C3" s="6">
         <v>1500</v>
@@ -950,10 +1149,10 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="C4" s="6">
         <v>1500</v>
@@ -980,10 +1179,10 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>141</v>
       </c>
       <c r="C5" s="6">
         <v>1500</v>
@@ -1006,10 +1205,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>147</v>
       </c>
       <c r="C6" s="6">
         <v>1500</v>
@@ -1036,10 +1235,10 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="C7" s="6">
         <v>1000</v>
@@ -1066,10 +1265,10 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>119</v>
       </c>
       <c r="C8" s="6">
         <v>1500</v>
@@ -1096,7 +1295,10 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>120</v>
       </c>
       <c r="C9" s="6">
         <v>2000</v>
@@ -1119,10 +1321,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="C10" s="6">
         <v>1800</v>
@@ -1149,10 +1351,10 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>143</v>
       </c>
       <c r="C11" s="6">
         <v>1500</v>
@@ -1179,10 +1381,10 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>121</v>
       </c>
       <c r="C12" s="6">
         <v>3000</v>
@@ -1209,10 +1411,10 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>122</v>
       </c>
       <c r="C13" s="6">
         <v>2000</v>
@@ -1239,10 +1441,10 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>47</v>
+        <v>123</v>
       </c>
       <c r="C14" s="6">
         <v>1800</v>
@@ -1265,10 +1467,10 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>91</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="C15" s="6">
         <v>2500</v>
@@ -1295,10 +1497,10 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>124</v>
       </c>
       <c r="C16" s="6">
         <v>3000</v>
@@ -1325,10 +1527,10 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>148</v>
       </c>
       <c r="C17" s="6">
         <v>1500</v>
@@ -1355,10 +1557,10 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>137</v>
       </c>
       <c r="C18" s="6">
         <v>2000</v>
@@ -1385,10 +1587,10 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="C19" s="6">
         <v>1500</v>
@@ -1417,10 +1619,10 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>145</v>
       </c>
       <c r="C20" s="6">
         <v>1500</v>
@@ -1447,10 +1649,10 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>149</v>
       </c>
       <c r="C21" s="6">
         <v>1500</v>
@@ -1477,10 +1679,10 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="C22" s="6">
         <v>1500</v>
@@ -1509,10 +1711,10 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="C23" s="6">
         <v>1000</v>
@@ -1541,10 +1743,10 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="C24" s="6">
         <v>1500</v>
@@ -1571,10 +1773,10 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="C25" s="6">
         <v>3000</v>
@@ -1601,10 +1803,10 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C26" s="6">
         <v>2000</v>
@@ -1631,10 +1833,10 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>96</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="C27" s="6">
         <v>2500</v>
@@ -1661,10 +1863,10 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="C28" s="6">
         <v>2300</v>
@@ -1691,10 +1893,10 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="C29" s="6">
         <v>1500</v>
@@ -1720,7 +1922,7 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="C30" s="6">
         <v>1500</v>
@@ -1749,10 +1951,10 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="C31" s="6">
         <v>1500</v>
@@ -1781,10 +1983,10 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" t="s">
         <v>151</v>
-      </c>
-      <c r="B32" t="s">
-        <v>6</v>
       </c>
       <c r="C32" s="6">
         <v>1500</v>
@@ -1813,10 +2015,10 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" t="s">
         <v>152</v>
-      </c>
-      <c r="B33" t="s">
-        <v>9</v>
       </c>
       <c r="C33" s="6">
         <v>1500</v>
@@ -1843,10 +2045,10 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" t="s">
         <v>153</v>
-      </c>
-      <c r="B34" t="s">
-        <v>8</v>
       </c>
       <c r="C34" s="6">
         <v>1500</v>
@@ -1873,10 +2075,10 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>139</v>
+        <v>98</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="C35" s="6">
         <v>2000</v>
@@ -1905,10 +2107,10 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="C36" s="6">
         <v>2000</v>
@@ -1934,11 +2136,11 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>140</v>
+      <c r="A37" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="C37" s="6">
         <v>2000</v>
@@ -1967,10 +2169,10 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="C38" s="6">
         <v>2000</v>
@@ -1999,10 +2201,10 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" t="s">
         <v>154</v>
-      </c>
-      <c r="B39" t="s">
-        <v>10</v>
       </c>
       <c r="C39" s="6">
         <v>1500</v>
@@ -2031,10 +2233,10 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" t="s">
         <v>155</v>
-      </c>
-      <c r="B40" t="s">
-        <v>7</v>
       </c>
       <c r="C40" s="6">
         <v>1500</v>
@@ -2063,10 +2265,10 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="C41" s="6">
         <v>2000</v>
@@ -2095,10 +2297,10 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="C42" s="6">
         <v>1500</v>
@@ -2127,10 +2329,10 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>146</v>
       </c>
       <c r="C43" s="6">
         <v>1500</v>
@@ -2159,10 +2361,10 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>157</v>
       </c>
       <c r="C44" s="6">
         <v>1500</v>
@@ -2191,10 +2393,10 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>62</v>
+        <v>132</v>
       </c>
       <c r="C45" s="6">
         <v>2000</v>
@@ -2223,10 +2425,10 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>63</v>
+        <v>135</v>
       </c>
       <c r="C46" s="6">
         <v>2000</v>
@@ -2253,10 +2455,10 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>158</v>
       </c>
       <c r="C47" s="6">
         <v>1500</v>
@@ -2283,10 +2485,10 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>144</v>
+        <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>65</v>
+        <v>133</v>
       </c>
       <c r="C48" s="6">
         <v>2000</v>
@@ -3002,27 +3204,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="E1" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="F1" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3">
         <v>2000</v>
@@ -3037,12 +3239,12 @@
         <v>0.443</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3">
         <v>1200</v>
@@ -3057,12 +3259,12 @@
         <v>2.637</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3">
         <v>700</v>
@@ -3077,12 +3279,12 @@
         <v>5.4349999999999996</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3">
         <v>720</v>
@@ -3097,12 +3299,12 @@
         <v>1.429</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3">
         <v>1055</v>
@@ -3117,12 +3319,12 @@
         <v>1.53</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="B7" s="3">
         <v>2000</v>
@@ -3137,12 +3339,12 @@
         <v>0.77100000000000002</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="B8" s="3">
         <v>1357</v>
@@ -3162,7 +3364,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3">
         <v>1400</v>
@@ -3177,12 +3379,12 @@
         <v>0.97299999999999998</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3">
         <v>1043</v>
@@ -3191,7 +3393,7 @@
         <v>3.0049999999999999</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="E10" s="3">
         <v>6.1109999999999998</v>
@@ -3202,7 +3404,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="B11" s="3">
         <v>960</v>
@@ -3217,12 +3419,12 @@
         <v>9.6969999999999992</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="B12" s="3">
         <v>850</v>
@@ -3242,7 +3444,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="B13" s="3">
         <v>411</v>
@@ -3257,12 +3459,12 @@
         <v>13.286</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="B14" s="3">
         <v>386.8</v>
@@ -3277,12 +3479,12 @@
         <v>1.502</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="B15" s="3">
         <v>800</v>
@@ -3297,12 +3499,12 @@
         <v>2.476</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="B16" s="3">
         <v>458</v>
@@ -3317,12 +3519,12 @@
         <v>16.105</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="B17" s="3">
         <v>371</v>
@@ -3337,12 +3539,12 @@
         <v>4.6879999999999997</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="B18" s="3">
         <v>1073</v>
@@ -3357,12 +3559,12 @@
         <v>1.9630000000000001</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="B19" s="3">
         <v>566</v>
@@ -3382,7 +3584,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="B20" s="3">
         <v>400</v>
@@ -3397,12 +3599,12 @@
         <v>18.148</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="B21" s="3">
         <v>368.3</v>
@@ -3414,15 +3616,15 @@
         <v>4.1139999999999999</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="B22" s="3">
         <v>847</v>
@@ -3437,7 +3639,7 @@
         <v>5.3650000000000002</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -3460,7 +3662,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3">
         <v>9.718</v>
@@ -3469,7 +3671,7 @@
         <v>22.626000000000001</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="E1" s="3">
         <v>192.71</v>
@@ -3477,7 +3679,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3">
         <v>23.07</v>
@@ -3489,29 +3691,29 @@
         <v>29.03</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3">
         <v>16.157</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3">
         <v>67.959999999999994</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3">
         <v>14.779</v>
@@ -3520,7 +3722,7 @@
         <v>22.710999999999999</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="E4" s="3">
         <v>205.79</v>
@@ -3528,7 +3730,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3">
         <v>15.750999999999999</v>
@@ -3537,7 +3739,7 @@
         <v>21.155000000000001</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="E5" s="3">
         <v>101.14</v>
@@ -3545,7 +3747,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="B6" s="3">
         <v>18.239999999999998</v>
@@ -3557,12 +3759,12 @@
         <v>32.86</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="B7" s="3">
         <v>13.805999999999999</v>
@@ -3571,7 +3773,7 @@
         <v>19.215</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="E7" s="3">
         <v>83.01</v>
@@ -3579,24 +3781,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3">
         <v>18.736999999999998</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="D8" s="3">
         <v>141.38</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>13.444000000000001</v>
@@ -3605,7 +3807,7 @@
         <v>33.866</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="E9" s="3">
         <v>349.17</v>
@@ -3613,7 +3815,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3">
         <v>10.59</v>
@@ -3622,7 +3824,7 @@
         <v>21.039000000000001</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="E10" s="3">
         <v>172.28</v>
@@ -3630,7 +3832,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3">
         <v>9.798</v>
@@ -3639,7 +3841,7 @@
         <v>13.430999999999999</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="E11" s="3">
         <v>131.13</v>
@@ -3647,7 +3849,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="B12" s="3">
         <v>16.920999999999999</v>
@@ -3656,7 +3858,7 @@
         <v>41.652999999999999</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="E12" s="3">
         <v>427.2</v>
@@ -3664,24 +3866,24 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="B13" s="3">
         <v>30.408000000000001</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
       <c r="D13" s="3">
         <v>137.08000000000001</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>121</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>18.611000000000001</v>
@@ -3698,7 +3900,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B15" s="3">
         <v>9.0690000000000008</v>
@@ -3710,7 +3912,7 @@
         <v>1.25</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3738,12 +3940,2343 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>16.042999999999999</v>
+      </c>
+      <c r="C2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D2">
+        <v>190.6</v>
+      </c>
+      <c r="E2">
+        <v>45.99</v>
+      </c>
+      <c r="F2">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="G2">
+        <v>98.6</v>
+      </c>
+      <c r="H2">
+        <v>111.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>30.07</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3">
+        <v>305.3</v>
+      </c>
+      <c r="E3">
+        <v>48.72</v>
+      </c>
+      <c r="F3">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="G3">
+        <v>145.5</v>
+      </c>
+      <c r="H3">
+        <v>184.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>44.097000000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.152</v>
+      </c>
+      <c r="D4">
+        <v>369.8</v>
+      </c>
+      <c r="E4">
+        <v>42.48</v>
+      </c>
+      <c r="F4">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="G4">
+        <v>200</v>
+      </c>
+      <c r="H4">
+        <v>231.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5">
+        <v>58.122999999999998</v>
+      </c>
+      <c r="C5">
+        <v>0.2</v>
+      </c>
+      <c r="D5">
+        <v>425.1</v>
+      </c>
+      <c r="E5">
+        <v>37.96</v>
+      </c>
+      <c r="F5">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="G5">
+        <v>255</v>
+      </c>
+      <c r="H5">
+        <v>272.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6">
+        <v>72.150000000000006</v>
+      </c>
+      <c r="C6">
+        <v>0.252</v>
+      </c>
+      <c r="D6">
+        <v>469.7</v>
+      </c>
+      <c r="E6">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="F6">
+        <v>0.27</v>
+      </c>
+      <c r="G6">
+        <v>313</v>
+      </c>
+      <c r="H6">
+        <v>309.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7">
+        <v>86.177000000000007</v>
+      </c>
+      <c r="C7">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="D7">
+        <v>507.6</v>
+      </c>
+      <c r="E7">
+        <v>30.25</v>
+      </c>
+      <c r="F7">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="G7">
+        <v>371</v>
+      </c>
+      <c r="H7">
+        <v>341.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8">
+        <v>100.20399999999999</v>
+      </c>
+      <c r="C8">
+        <v>0.35</v>
+      </c>
+      <c r="D8">
+        <v>540.20000000000005</v>
+      </c>
+      <c r="E8">
+        <v>27.4</v>
+      </c>
+      <c r="F8">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="G8">
+        <v>428</v>
+      </c>
+      <c r="H8">
+        <v>371.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9">
+        <v>114.23099999999999</v>
+      </c>
+      <c r="C9">
+        <v>0.4</v>
+      </c>
+      <c r="D9">
+        <v>568.70000000000005</v>
+      </c>
+      <c r="E9">
+        <v>24.9</v>
+      </c>
+      <c r="F9">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="G9">
+        <v>486</v>
+      </c>
+      <c r="H9">
+        <v>398.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10">
+        <v>128.25800000000001</v>
+      </c>
+      <c r="C10">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="D10">
+        <v>594.6</v>
+      </c>
+      <c r="E10">
+        <v>22.9</v>
+      </c>
+      <c r="F10">
+        <v>0.252</v>
+      </c>
+      <c r="G10">
+        <v>544</v>
+      </c>
+      <c r="H10">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11">
+        <v>142.285</v>
+      </c>
+      <c r="C11">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="D11">
+        <v>617.70000000000005</v>
+      </c>
+      <c r="E11">
+        <v>21.1</v>
+      </c>
+      <c r="F11">
+        <v>0.247</v>
+      </c>
+      <c r="G11">
+        <v>600</v>
+      </c>
+      <c r="H11">
+        <v>447.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12">
+        <v>58.122999999999998</v>
+      </c>
+      <c r="C12">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="D12">
+        <v>408.1</v>
+      </c>
+      <c r="E12">
+        <v>36.479999999999997</v>
+      </c>
+      <c r="F12">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="G12">
+        <v>262.7</v>
+      </c>
+      <c r="H12">
+        <v>261.39999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13">
+        <v>114.23099999999999</v>
+      </c>
+      <c r="C13">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="D13">
+        <v>544</v>
+      </c>
+      <c r="E13">
+        <v>25.68</v>
+      </c>
+      <c r="F13">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="G13">
+        <v>468</v>
+      </c>
+      <c r="H13">
+        <v>372.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14">
+        <v>70.134</v>
+      </c>
+      <c r="C14">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="D14">
+        <v>511.8</v>
+      </c>
+      <c r="E14">
+        <v>45.02</v>
+      </c>
+      <c r="F14">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="G14">
+        <v>258</v>
+      </c>
+      <c r="H14">
+        <v>322.39999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>84.161000000000001</v>
+      </c>
+      <c r="C15">
+        <v>0.21</v>
+      </c>
+      <c r="D15">
+        <v>553.6</v>
+      </c>
+      <c r="E15">
+        <v>40.729999999999997</v>
+      </c>
+      <c r="F15">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="G15">
+        <v>308</v>
+      </c>
+      <c r="H15">
+        <v>353.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16">
+        <v>84.161000000000001</v>
+      </c>
+      <c r="C16">
+        <v>0.23</v>
+      </c>
+      <c r="D16">
+        <v>532.79999999999995</v>
+      </c>
+      <c r="E16">
+        <v>37.85</v>
+      </c>
+      <c r="F16">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="G16">
+        <v>319</v>
+      </c>
+      <c r="H16">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17">
+        <v>98.188000000000002</v>
+      </c>
+      <c r="C17">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="D17">
+        <v>572.20000000000005</v>
+      </c>
+      <c r="E17">
+        <v>34.71</v>
+      </c>
+      <c r="F17">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="G17">
+        <v>368</v>
+      </c>
+      <c r="H17">
+        <v>374.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18">
+        <v>28.053999999999998</v>
+      </c>
+      <c r="C18">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="D18">
+        <v>282.3</v>
+      </c>
+      <c r="E18">
+        <v>50.4</v>
+      </c>
+      <c r="F18">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="G18">
+        <v>131</v>
+      </c>
+      <c r="H18">
+        <v>169.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>42.081000000000003</v>
+      </c>
+      <c r="C19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D19">
+        <v>365.6</v>
+      </c>
+      <c r="E19">
+        <v>46.65</v>
+      </c>
+      <c r="F19">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="G19">
+        <v>188.4</v>
+      </c>
+      <c r="H19">
+        <v>225.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B20">
+        <v>56.107999999999997</v>
+      </c>
+      <c r="C20">
+        <v>0.191</v>
+      </c>
+      <c r="D20">
+        <v>420</v>
+      </c>
+      <c r="E20">
+        <v>40.43</v>
+      </c>
+      <c r="F20">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="G20">
+        <v>239.3</v>
+      </c>
+      <c r="H20">
+        <v>266.89999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21">
+        <v>56.107999999999997</v>
+      </c>
+      <c r="C21">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="D21">
+        <v>435.6</v>
+      </c>
+      <c r="E21">
+        <v>42.43</v>
+      </c>
+      <c r="F21">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="G21">
+        <v>233.8</v>
+      </c>
+      <c r="H21">
+        <v>276.89999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22">
+        <v>56.107999999999997</v>
+      </c>
+      <c r="C22">
+        <v>0.218</v>
+      </c>
+      <c r="D22">
+        <v>428.6</v>
+      </c>
+      <c r="E22">
+        <v>41</v>
+      </c>
+      <c r="F22">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G22">
+        <v>237.7</v>
+      </c>
+      <c r="H22">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23">
+        <v>84.161000000000001</v>
+      </c>
+      <c r="C23">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D23">
+        <v>504</v>
+      </c>
+      <c r="E23">
+        <v>31.4</v>
+      </c>
+      <c r="F23">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="G23">
+        <v>354</v>
+      </c>
+      <c r="H23">
+        <v>336.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>184</v>
+      </c>
+      <c r="B24">
+        <v>56.107999999999997</v>
+      </c>
+      <c r="C24">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="D24">
+        <v>417.9</v>
+      </c>
+      <c r="E24">
+        <v>40</v>
+      </c>
+      <c r="F24">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G24">
+        <v>238.9</v>
+      </c>
+      <c r="H24">
+        <v>266.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>54.091999999999999</v>
+      </c>
+      <c r="C25">
+        <v>0.19</v>
+      </c>
+      <c r="D25">
+        <v>425.2</v>
+      </c>
+      <c r="E25">
+        <v>42.77</v>
+      </c>
+      <c r="F25">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="G25">
+        <v>220.4</v>
+      </c>
+      <c r="H25">
+        <v>268.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26">
+        <v>82.144999999999996</v>
+      </c>
+      <c r="C26">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="D26">
+        <v>560.4</v>
+      </c>
+      <c r="E26">
+        <v>43.5</v>
+      </c>
+      <c r="F26">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="G26">
+        <v>291</v>
+      </c>
+      <c r="H26">
+        <v>356.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>26.038</v>
+      </c>
+      <c r="C27">
+        <v>0.187</v>
+      </c>
+      <c r="D27">
+        <v>308.3</v>
+      </c>
+      <c r="E27">
+        <v>61.39</v>
+      </c>
+      <c r="F27">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="G27">
+        <v>113</v>
+      </c>
+      <c r="H27">
+        <v>189.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>78.114000000000004</v>
+      </c>
+      <c r="C28">
+        <v>0.21</v>
+      </c>
+      <c r="D28">
+        <v>562.20000000000005</v>
+      </c>
+      <c r="E28">
+        <v>48.98</v>
+      </c>
+      <c r="F28">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="G28">
+        <v>259</v>
+      </c>
+      <c r="H28">
+        <v>353.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>92.141000000000005</v>
+      </c>
+      <c r="C29">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="D29">
+        <v>591.79999999999995</v>
+      </c>
+      <c r="E29">
+        <v>41.06</v>
+      </c>
+      <c r="F29">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="G29">
+        <v>316</v>
+      </c>
+      <c r="H29">
+        <v>383.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>106.167</v>
+      </c>
+      <c r="C30">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="D30">
+        <v>617.20000000000005</v>
+      </c>
+      <c r="E30">
+        <v>36.06</v>
+      </c>
+      <c r="F30">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G30">
+        <v>374</v>
+      </c>
+      <c r="H30">
+        <v>409.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>186</v>
+      </c>
+      <c r="B31">
+        <v>120.194</v>
+      </c>
+      <c r="C31">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="D31">
+        <v>631.1</v>
+      </c>
+      <c r="E31">
+        <v>32.090000000000003</v>
+      </c>
+      <c r="F31">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="G31">
+        <v>427</v>
+      </c>
+      <c r="H31">
+        <v>425.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>187</v>
+      </c>
+      <c r="B32">
+        <v>106.167</v>
+      </c>
+      <c r="C32">
+        <v>0.31</v>
+      </c>
+      <c r="D32">
+        <v>630.29999999999995</v>
+      </c>
+      <c r="E32">
+        <v>37.340000000000003</v>
+      </c>
+      <c r="F32">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G32">
+        <v>369</v>
+      </c>
+      <c r="H32">
+        <v>417.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33">
+        <v>106.167</v>
+      </c>
+      <c r="C33">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="D33">
+        <v>617.1</v>
+      </c>
+      <c r="E33">
+        <v>35.36</v>
+      </c>
+      <c r="F33">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="G33">
+        <v>376</v>
+      </c>
+      <c r="H33">
+        <v>412.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>189</v>
+      </c>
+      <c r="B34">
+        <v>106.167</v>
+      </c>
+      <c r="C34">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="D34">
+        <v>616.20000000000005</v>
+      </c>
+      <c r="E34">
+        <v>35.11</v>
+      </c>
+      <c r="F34">
+        <v>0.26</v>
+      </c>
+      <c r="G34">
+        <v>379</v>
+      </c>
+      <c r="H34">
+        <v>411.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35">
+        <v>104.152</v>
+      </c>
+      <c r="C35">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="D35">
+        <v>636</v>
+      </c>
+      <c r="E35">
+        <v>38.4</v>
+      </c>
+      <c r="F35">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="G35">
+        <v>352</v>
+      </c>
+      <c r="H35">
+        <v>418.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>190</v>
+      </c>
+      <c r="B36">
+        <v>128.17400000000001</v>
+      </c>
+      <c r="C36">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="D36">
+        <v>748.4</v>
+      </c>
+      <c r="E36">
+        <v>40.51</v>
+      </c>
+      <c r="F36">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="G36">
+        <v>413</v>
+      </c>
+      <c r="H36">
+        <v>491.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>191</v>
+      </c>
+      <c r="B37">
+        <v>154.21100000000001</v>
+      </c>
+      <c r="C37">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="D37">
+        <v>789.3</v>
+      </c>
+      <c r="E37">
+        <v>38.5</v>
+      </c>
+      <c r="F37">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="G37">
+        <v>502</v>
+      </c>
+      <c r="H37">
+        <v>528.20000000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38">
+        <v>30.026</v>
+      </c>
+      <c r="C38">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="D38">
+        <v>408</v>
+      </c>
+      <c r="E38">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="F38">
+        <v>0.223</v>
+      </c>
+      <c r="G38">
+        <v>115</v>
+      </c>
+      <c r="H38">
+        <v>254.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>44.052999999999997</v>
+      </c>
+      <c r="C39">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="D39">
+        <v>466</v>
+      </c>
+      <c r="E39">
+        <v>55.5</v>
+      </c>
+      <c r="F39">
+        <v>0.221</v>
+      </c>
+      <c r="G39">
+        <v>154</v>
+      </c>
+      <c r="H39">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>209</v>
+      </c>
+      <c r="B40">
+        <v>74.078999999999994</v>
+      </c>
+      <c r="C40">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="D40">
+        <v>506.6</v>
+      </c>
+      <c r="E40">
+        <v>47.5</v>
+      </c>
+      <c r="F40">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="G40">
+        <v>228</v>
+      </c>
+      <c r="H40">
+        <v>330.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>210</v>
+      </c>
+      <c r="B41">
+        <v>88.105999999999995</v>
+      </c>
+      <c r="C41">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="D41">
+        <v>523.29999999999995</v>
+      </c>
+      <c r="E41">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="F41">
+        <v>0.255</v>
+      </c>
+      <c r="G41">
+        <v>286</v>
+      </c>
+      <c r="H41">
+        <v>350.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>192</v>
+      </c>
+      <c r="B42">
+        <v>58.08</v>
+      </c>
+      <c r="C42">
+        <v>0.307</v>
+      </c>
+      <c r="D42">
+        <v>508.2</v>
+      </c>
+      <c r="E42">
+        <v>47.01</v>
+      </c>
+      <c r="F42">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G42">
+        <v>209</v>
+      </c>
+      <c r="H42">
+        <v>329.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>211</v>
+      </c>
+      <c r="B43">
+        <v>72.106999999999999</v>
+      </c>
+      <c r="C43">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="D43">
+        <v>535.5</v>
+      </c>
+      <c r="E43">
+        <v>41.5</v>
+      </c>
+      <c r="F43">
+        <v>0.249</v>
+      </c>
+      <c r="G43">
+        <v>267</v>
+      </c>
+      <c r="H43">
+        <v>352.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>212</v>
+      </c>
+      <c r="B44">
+        <v>74.123000000000005</v>
+      </c>
+      <c r="C44">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="D44">
+        <v>466.7</v>
+      </c>
+      <c r="E44">
+        <v>36.4</v>
+      </c>
+      <c r="F44">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G44">
+        <v>280</v>
+      </c>
+      <c r="H44">
+        <v>307.60000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>213</v>
+      </c>
+      <c r="B45">
+        <v>88.15</v>
+      </c>
+      <c r="C45">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="D45">
+        <v>497.1</v>
+      </c>
+      <c r="E45">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="F45">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="G45">
+        <v>329</v>
+      </c>
+      <c r="H45">
+        <v>328.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <v>32.042000000000002</v>
+      </c>
+      <c r="C46">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="D46">
+        <v>512.6</v>
+      </c>
+      <c r="E46">
+        <v>80.97</v>
+      </c>
+      <c r="F46">
+        <v>0.224</v>
+      </c>
+      <c r="G46">
+        <v>118</v>
+      </c>
+      <c r="H46">
+        <v>337.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47">
+        <v>46.069000000000003</v>
+      </c>
+      <c r="C47">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="D47">
+        <v>513.9</v>
+      </c>
+      <c r="E47">
+        <v>61.48</v>
+      </c>
+      <c r="F47">
+        <v>0.24</v>
+      </c>
+      <c r="G47">
+        <v>167</v>
+      </c>
+      <c r="H47">
+        <v>351.4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>193</v>
+      </c>
+      <c r="B48">
+        <v>60.095999999999997</v>
+      </c>
+      <c r="C48">
+        <v>0.622</v>
+      </c>
+      <c r="D48">
+        <v>536.79999999999995</v>
+      </c>
+      <c r="E48">
+        <v>51.75</v>
+      </c>
+      <c r="F48">
+        <v>0.254</v>
+      </c>
+      <c r="G48">
+        <v>219</v>
+      </c>
+      <c r="H48">
+        <v>370.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>194</v>
+      </c>
+      <c r="B49">
+        <v>74.123000000000005</v>
+      </c>
+      <c r="C49">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="D49">
+        <v>563.1</v>
+      </c>
+      <c r="E49">
+        <v>44.23</v>
+      </c>
+      <c r="F49">
+        <v>0.26</v>
+      </c>
+      <c r="G49">
+        <v>275</v>
+      </c>
+      <c r="H49">
+        <v>390.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>195</v>
+      </c>
+      <c r="B50">
+        <v>102.17700000000001</v>
+      </c>
+      <c r="C50">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="D50">
+        <v>611.4</v>
+      </c>
+      <c r="E50">
+        <v>35.1</v>
+      </c>
+      <c r="F50">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G50">
+        <v>381</v>
+      </c>
+      <c r="H50">
+        <v>430.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51">
+        <v>60.095999999999997</v>
+      </c>
+      <c r="C51">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="D51">
+        <v>508.3</v>
+      </c>
+      <c r="E51">
+        <v>47.62</v>
+      </c>
+      <c r="F51">
+        <v>0.248</v>
+      </c>
+      <c r="G51">
+        <v>220</v>
+      </c>
+      <c r="H51">
+        <v>355.4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>197</v>
+      </c>
+      <c r="B52">
+        <v>94.113</v>
+      </c>
+      <c r="C52">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="D52">
+        <v>694.3</v>
+      </c>
+      <c r="E52">
+        <v>61.3</v>
+      </c>
+      <c r="F52">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="G52">
+        <v>229</v>
+      </c>
+      <c r="H52">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>214</v>
+      </c>
+      <c r="B53">
+        <v>62.067999999999998</v>
+      </c>
+      <c r="C53">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="D53">
+        <v>719.7</v>
+      </c>
+      <c r="E53">
+        <v>77</v>
+      </c>
+      <c r="F53">
+        <v>0.246</v>
+      </c>
+      <c r="G53">
+        <v>191</v>
+      </c>
+      <c r="H53">
+        <v>470.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>215</v>
+      </c>
+      <c r="B54">
+        <v>60.052999999999997</v>
+      </c>
+      <c r="C54">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="D54">
+        <v>592</v>
+      </c>
+      <c r="E54">
+        <v>57.86</v>
+      </c>
+      <c r="F54">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="G54">
+        <v>179.7</v>
+      </c>
+      <c r="H54">
+        <v>391.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>216</v>
+      </c>
+      <c r="B55">
+        <v>88.105999999999995</v>
+      </c>
+      <c r="C55">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="D55">
+        <v>615.70000000000005</v>
+      </c>
+      <c r="E55">
+        <v>40.64</v>
+      </c>
+      <c r="F55">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="G55">
+        <v>291.7</v>
+      </c>
+      <c r="H55">
+        <v>436.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>217</v>
+      </c>
+      <c r="B56">
+        <v>122.123</v>
+      </c>
+      <c r="C56">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="D56">
+        <v>751</v>
+      </c>
+      <c r="E56">
+        <v>44.7</v>
+      </c>
+      <c r="F56">
+        <v>0.246</v>
+      </c>
+      <c r="G56">
+        <v>344</v>
+      </c>
+      <c r="H56">
+        <v>522.4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>198</v>
+      </c>
+      <c r="B57">
+        <v>41.052999999999997</v>
+      </c>
+      <c r="C57">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="D57">
+        <v>545.5</v>
+      </c>
+      <c r="E57">
+        <v>48.3</v>
+      </c>
+      <c r="F57">
+        <v>0.184</v>
+      </c>
+      <c r="G57">
+        <v>173</v>
+      </c>
+      <c r="H57">
+        <v>354.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>199</v>
+      </c>
+      <c r="B58">
+        <v>31.056999999999999</v>
+      </c>
+      <c r="C58">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="D58">
+        <v>430.1</v>
+      </c>
+      <c r="E58">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="F58">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="G58">
+        <v>154</v>
+      </c>
+      <c r="H58">
+        <v>266.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>200</v>
+      </c>
+      <c r="B59">
+        <v>45.084000000000003</v>
+      </c>
+      <c r="C59">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="D59">
+        <v>456.2</v>
+      </c>
+      <c r="E59">
+        <v>56.2</v>
+      </c>
+      <c r="F59">
+        <v>0.307</v>
+      </c>
+      <c r="G59">
+        <v>207</v>
+      </c>
+      <c r="H59">
+        <v>289.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>201</v>
+      </c>
+      <c r="B60">
+        <v>61.04</v>
+      </c>
+      <c r="C60">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="D60">
+        <v>588.20000000000005</v>
+      </c>
+      <c r="E60">
+        <v>63.1</v>
+      </c>
+      <c r="F60">
+        <v>0.223</v>
+      </c>
+      <c r="G60">
+        <v>173</v>
+      </c>
+      <c r="H60">
+        <v>374.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>218</v>
+      </c>
+      <c r="B61">
+        <v>153.822</v>
+      </c>
+      <c r="C61">
+        <v>0.193</v>
+      </c>
+      <c r="D61">
+        <v>556.4</v>
+      </c>
+      <c r="E61">
+        <v>45.6</v>
+      </c>
+      <c r="F61">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="G61">
+        <v>276</v>
+      </c>
+      <c r="H61">
+        <v>349.8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62">
+        <v>119.377</v>
+      </c>
+      <c r="C62">
+        <v>0.222</v>
+      </c>
+      <c r="D62">
+        <v>536.4</v>
+      </c>
+      <c r="E62">
+        <v>54.72</v>
+      </c>
+      <c r="F62">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="G62">
+        <v>239</v>
+      </c>
+      <c r="H62">
+        <v>334.3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>202</v>
+      </c>
+      <c r="B63">
+        <v>84.932000000000002</v>
+      </c>
+      <c r="C63">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="D63">
+        <v>510</v>
+      </c>
+      <c r="E63">
+        <v>60.8</v>
+      </c>
+      <c r="F63">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="G63">
+        <v>185</v>
+      </c>
+      <c r="H63">
+        <v>312.89999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>219</v>
+      </c>
+      <c r="B64">
+        <v>50.488</v>
+      </c>
+      <c r="C64">
+        <v>0.153</v>
+      </c>
+      <c r="D64">
+        <v>416.3</v>
+      </c>
+      <c r="E64">
+        <v>66.8</v>
+      </c>
+      <c r="F64">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="G64">
+        <v>143</v>
+      </c>
+      <c r="H64">
+        <v>249.1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>220</v>
+      </c>
+      <c r="B65">
+        <v>64.513999999999996</v>
+      </c>
+      <c r="C65">
+        <v>0.19</v>
+      </c>
+      <c r="D65">
+        <v>460.4</v>
+      </c>
+      <c r="E65">
+        <v>52.7</v>
+      </c>
+      <c r="F65">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G65">
+        <v>200</v>
+      </c>
+      <c r="H65">
+        <v>285.39999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66">
+        <v>112.55800000000001</v>
+      </c>
+      <c r="C66">
+        <v>0.25</v>
+      </c>
+      <c r="D66">
+        <v>632.4</v>
+      </c>
+      <c r="E66">
+        <v>45.2</v>
+      </c>
+      <c r="F66">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="G66">
+        <v>308</v>
+      </c>
+      <c r="H66">
+        <v>404.9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>203</v>
+      </c>
+      <c r="B67">
+        <v>102.03</v>
+      </c>
+      <c r="C67">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="D67">
+        <v>374.2</v>
+      </c>
+      <c r="E67">
+        <v>40.6</v>
+      </c>
+      <c r="F67">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="G67">
+        <v>198</v>
+      </c>
+      <c r="H67">
+        <v>247.1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>204</v>
+      </c>
+      <c r="B68">
+        <v>39.948</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>150.9</v>
+      </c>
+      <c r="E68">
+        <v>48.98</v>
+      </c>
+      <c r="F68">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="G68">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="H68">
+        <v>87.3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>205</v>
+      </c>
+      <c r="B69">
+        <v>83.8</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>209.4</v>
+      </c>
+      <c r="E69">
+        <v>55.02</v>
+      </c>
+      <c r="F69">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="G69">
+        <v>91.2</v>
+      </c>
+      <c r="H69">
+        <v>119.8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>206</v>
+      </c>
+      <c r="B70">
+        <v>131.30000000000001</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>289.7</v>
+      </c>
+      <c r="E70">
+        <v>58.4</v>
+      </c>
+      <c r="F70">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="G70">
+        <v>118</v>
+      </c>
+      <c r="H70">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>221</v>
+      </c>
+      <c r="B71">
+        <v>4.0030000000000001</v>
+      </c>
+      <c r="C71" t="s">
+        <v>207</v>
+      </c>
+      <c r="D71">
+        <v>5.2</v>
+      </c>
+      <c r="E71">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="F71">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="G71">
+        <v>57.3</v>
+      </c>
+      <c r="H71">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>89</v>
+      </c>
+      <c r="B72">
+        <v>2.016</v>
+      </c>
+      <c r="C72" t="s">
+        <v>208</v>
+      </c>
+      <c r="D72">
+        <v>33.19</v>
+      </c>
+      <c r="E72">
+        <v>13.13</v>
+      </c>
+      <c r="F72">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="G72">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="H72">
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73">
+        <v>31.998999999999999</v>
+      </c>
+      <c r="C73">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D73">
+        <v>154.6</v>
+      </c>
+      <c r="E73">
+        <v>50.43</v>
+      </c>
+      <c r="F73">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="G73">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="H73">
+        <v>90.2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>159</v>
+      </c>
+      <c r="B74">
+        <v>28.013999999999999</v>
+      </c>
+      <c r="C74">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D74">
+        <v>126.2</v>
+      </c>
+      <c r="E74">
+        <v>34</v>
+      </c>
+      <c r="F74">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="G74">
+        <v>89.2</v>
+      </c>
+      <c r="H74">
+        <v>77.3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>15</v>
+      </c>
+      <c r="B75">
+        <v>28.850999999999999</v>
+      </c>
+      <c r="C75">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D75">
+        <v>132.19999999999999</v>
+      </c>
+      <c r="E75">
+        <v>37.450000000000003</v>
+      </c>
+      <c r="F75">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="G75">
+        <v>84.8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76">
+        <v>70.905000000000001</v>
+      </c>
+      <c r="C76">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="D76">
+        <v>417.2</v>
+      </c>
+      <c r="E76">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="F76">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="G76">
+        <v>124</v>
+      </c>
+      <c r="H76">
+        <v>239.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>91</v>
+      </c>
+      <c r="B77">
+        <v>28.01</v>
+      </c>
+      <c r="C77">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="D77">
+        <v>132.9</v>
+      </c>
+      <c r="E77">
+        <v>34.99</v>
+      </c>
+      <c r="F77">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="G77">
+        <v>93.4</v>
+      </c>
+      <c r="H77">
+        <v>81.7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>92</v>
+      </c>
+      <c r="B78">
+        <v>44.01</v>
+      </c>
+      <c r="C78">
+        <v>0.224</v>
+      </c>
+      <c r="D78">
+        <v>304.2</v>
+      </c>
+      <c r="E78">
+        <v>73.83</v>
+      </c>
+      <c r="F78">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="G78">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>93</v>
+      </c>
+      <c r="B79">
+        <v>76.143000000000001</v>
+      </c>
+      <c r="C79">
+        <v>0.111</v>
+      </c>
+      <c r="D79">
+        <v>552</v>
+      </c>
+      <c r="E79">
+        <v>79</v>
+      </c>
+      <c r="F79">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G79">
+        <v>160</v>
+      </c>
+      <c r="H79">
+        <v>319.39999999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>94</v>
+      </c>
+      <c r="B80">
+        <v>34.082000000000001</v>
+      </c>
+      <c r="C80">
+        <v>9.4E-2</v>
+      </c>
+      <c r="D80">
+        <v>373.5</v>
+      </c>
+      <c r="E80">
+        <v>89.63</v>
+      </c>
+      <c r="F80">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="G80">
+        <v>98.5</v>
+      </c>
+      <c r="H80">
+        <v>212.8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>101</v>
+      </c>
+      <c r="B81">
+        <v>64.064999999999998</v>
+      </c>
+      <c r="C81">
+        <v>0.245</v>
+      </c>
+      <c r="D81">
+        <v>430.8</v>
+      </c>
+      <c r="E81">
+        <v>78.84</v>
+      </c>
+      <c r="F81">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="G81">
+        <v>122</v>
+      </c>
+      <c r="H81">
+        <v>263.10000000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>102</v>
+      </c>
+      <c r="B82">
+        <v>80.063999999999993</v>
+      </c>
+      <c r="C82">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="D82">
+        <v>490.9</v>
+      </c>
+      <c r="E82">
+        <v>82.1</v>
+      </c>
+      <c r="F82">
+        <v>0.255</v>
+      </c>
+      <c r="G82">
+        <v>127</v>
+      </c>
+      <c r="H82">
+        <v>317.89999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>98</v>
+      </c>
+      <c r="B83">
+        <v>30.006</v>
+      </c>
+      <c r="C83">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="D83">
+        <v>180.2</v>
+      </c>
+      <c r="E83">
+        <v>64.8</v>
+      </c>
+      <c r="F83">
+        <v>0.251</v>
+      </c>
+      <c r="G83">
+        <v>58</v>
+      </c>
+      <c r="H83">
+        <v>121.4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>97</v>
+      </c>
+      <c r="B84">
+        <v>44.012999999999998</v>
+      </c>
+      <c r="C84">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="D84">
+        <v>309.60000000000002</v>
+      </c>
+      <c r="E84">
+        <v>72.45</v>
+      </c>
+      <c r="F84">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="G84">
+        <v>97.4</v>
+      </c>
+      <c r="H84">
+        <v>184.7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>95</v>
+      </c>
+      <c r="B85">
+        <v>36.460999999999999</v>
+      </c>
+      <c r="C85">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="D85">
+        <v>324.7</v>
+      </c>
+      <c r="E85">
+        <v>83.1</v>
+      </c>
+      <c r="F85">
+        <v>0.249</v>
+      </c>
+      <c r="G85">
+        <v>81</v>
+      </c>
+      <c r="H85">
+        <v>188.2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>96</v>
+      </c>
+      <c r="B86">
+        <v>27.026</v>
+      </c>
+      <c r="C86">
+        <v>0.41</v>
+      </c>
+      <c r="D86">
+        <v>456.7</v>
+      </c>
+      <c r="E86">
+        <v>53.9</v>
+      </c>
+      <c r="F86">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="G86">
+        <v>139</v>
+      </c>
+      <c r="H86">
+        <v>298.89999999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>103</v>
+      </c>
+      <c r="B87">
+        <v>18.015000000000001</v>
+      </c>
+      <c r="C87">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="D87">
+        <v>647.1</v>
+      </c>
+      <c r="E87">
+        <v>220.55</v>
+      </c>
+      <c r="F87">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="G87">
+        <v>55.9</v>
+      </c>
+      <c r="H87">
+        <v>373.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>16</v>
+      </c>
+      <c r="B88">
+        <v>17.030999999999999</v>
+      </c>
+      <c r="C88">
+        <v>0.253</v>
+      </c>
+      <c r="D88">
+        <v>405.7</v>
+      </c>
+      <c r="E88">
+        <v>112.8</v>
+      </c>
+      <c r="F88">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="G88">
+        <v>72.5</v>
+      </c>
+      <c r="H88">
+        <v>239.7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>222</v>
+      </c>
+      <c r="B89">
+        <v>63.012999999999998</v>
+      </c>
+      <c r="C89">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="D89">
+        <v>520</v>
+      </c>
+      <c r="E89">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="F89">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="G89">
+        <v>145</v>
+      </c>
+      <c r="H89">
+        <v>356.2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>223</v>
+      </c>
+      <c r="B90">
+        <v>98.08</v>
+      </c>
+      <c r="D90">
+        <v>924</v>
+      </c>
+      <c r="E90">
+        <v>64</v>
+      </c>
+      <c r="F90">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="G90">
+        <v>177</v>
+      </c>
+      <c r="H90">
+        <v>610</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>